<commit_message>
Caso y procedimiento de prueba 1.2
</commit_message>
<xml_diff>
--- a/pruebas/Casos_de_prueba.xlsx
+++ b/pruebas/Casos_de_prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="299" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="426" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>Procedimiento de Prueba: </t>
+  </si>
+  <si>
+    <t>1- Ingresar a la pantalla de identificación.</t>
+  </si>
+  <si>
+    <t>2- Ingresar Nombre de Usuario y contraseña</t>
+  </si>
+  <si>
+    <t>3- Presionar botón identificarse</t>
+  </si>
   <si>
     <t>Código</t>
   </si>
@@ -57,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -79,6 +91,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,9 +150,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -163,7 +191,7 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -177,52 +205,94 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5344129554656"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="6" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>